<commit_message>
frame work data setup
</commit_message>
<xml_diff>
--- a/src/main/java/Data/TestSuite1/Data.xlsx
+++ b/src/main/java/Data/TestSuite1/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="14295" windowHeight="4620"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="11310" windowHeight="3975"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,16 +12,23 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>TC_Name</t>
   </si>
   <si>
     <t>Destination</t>
+  </si>
+  <si>
+    <t>enterDetailsHomePage</t>
+  </si>
+  <si>
+    <t>Mum</t>
   </si>
 </sst>
 </file>
@@ -353,15 +360,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" customWidth="1"/>
@@ -375,6 +382,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>